<commit_message>
Added move email to folder feature
</commit_message>
<xml_diff>
--- a/Collate hour worked from employees ReFramework/Config/Config.xlsx
+++ b/Collate hour worked from employees ReFramework/Config/Config.xlsx
@@ -8,21 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Collate hour worked from employees ReFramework\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D391FE22-09F7-4AED-A8A8-47BCEC2ECCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED015AF-C312-4D57-99E2-B762A5772D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20760" yWindow="2835" windowWidth="16545" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1335" yWindow="1875" windowWidth="16020" windowHeight="11970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +188,18 @@
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>Add hours email folder</t>
+  </si>
+  <si>
+    <t>Update employee payroll details folder</t>
+  </si>
+  <si>
+    <t>HR automation\Add hours</t>
+  </si>
+  <si>
+    <t>HR automation\Update employee payroll details</t>
   </si>
 </sst>
 </file>
@@ -556,7 +578,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -710,8 +732,22 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed issue with config file not being found in when the process was run in UiPath Orchestrator
</commit_message>
<xml_diff>
--- a/Collate hour worked from employees ReFramework/Config/Config.xlsx
+++ b/Collate hour worked from employees ReFramework/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Collate hour worked from employees ReFramework\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8778B664-E96B-4781-BB57-43B29CFAE918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3C410A-3D7A-4932-BB1B-427878E41EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -196,10 +196,19 @@
     <t>HR automation\Update employee payroll details</t>
   </si>
   <si>
-    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Database\\Collate hour worked from employees ReFramework\\Employee table template.xlsx</t>
-  </si>
-  <si>
-    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Database\\Collate hour worked from employees ReFramework\\</t>
+    <t>EmployeeTableName</t>
+  </si>
+  <si>
+    <t>EmployeeTableAssetName</t>
+  </si>
+  <si>
+    <t>Asset name used to set the asset value that is used later on in the automation</t>
+  </si>
+  <si>
+    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Collate hour worked from employees ReFramework\\Database\\</t>
+  </si>
+  <si>
+    <t>C:\\Users\\premal\\Google Drive\\QAC projects\\HR automation\\automation\\HR-Payroll-automation\\Collate hour worked from employees ReFramework\\Database\\Employee table template.xlsx</t>
   </si>
 </sst>
 </file>
@@ -578,7 +587,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -639,7 +648,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -650,7 +659,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>41</v>
@@ -748,7 +757,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>